<commit_message>
dodan u user podaci za izvjesce
</commit_message>
<xml_diff>
--- a/app/assets/Sablona_za_nenaplacena_potrazivanja.xlsx
+++ b/app/assets/Sablona_za_nenaplacena_potrazivanja.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesenovic/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesenovic/RubymineProjects/untitled1/public/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-1880" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Zaglavlje" sheetId="1" r:id="rId1"/>
@@ -26,65 +26,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
-  <si>
-    <t>Datum_od</t>
-  </si>
-  <si>
-    <t>Datum_do</t>
-  </si>
-  <si>
-    <t>Oib</t>
-  </si>
-  <si>
-    <t>Naziv</t>
-  </si>
-  <si>
-    <t>Mjesto</t>
-  </si>
-  <si>
-    <t>Ulica</t>
-  </si>
-  <si>
-    <t>Broj</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>sastavio_ime</t>
-  </si>
-  <si>
-    <t>sastavio_prezime</t>
-  </si>
-  <si>
-    <t>sastavio_tel</t>
-  </si>
-  <si>
-    <t>sastavio_fax</t>
-  </si>
-  <si>
-    <t>sastavio_email</t>
-  </si>
-  <si>
     <t>na_dan</t>
   </si>
   <si>
     <t>nisu_naplaceni_do</t>
   </si>
   <si>
-    <t>Oznaka_poreznog_broja</t>
-  </si>
-  <si>
-    <t>Porezni_broj</t>
-  </si>
-  <si>
-    <t>Naziv_kupca</t>
-  </si>
-  <si>
-    <t>Broj_izdanog_racuna</t>
-  </si>
-  <si>
     <t>datum_izdanog_racuna</t>
   </si>
   <si>
@@ -100,48 +52,55 @@
     <t>porezni_broj_kupca</t>
   </si>
   <si>
-    <t>Cactus Code d.o.o.</t>
-  </si>
-  <si>
-    <t>Zagreb</t>
-  </si>
-  <si>
-    <t>Velika Cesta</t>
-  </si>
-  <si>
-    <t>hrvoje.jesenovic@gmail.com</t>
-  </si>
-  <si>
-    <t>Hrvoje</t>
-  </si>
-  <si>
-    <t>Jesenović</t>
-  </si>
-  <si>
-    <t>012222</t>
-  </si>
-  <si>
-    <t>01222</t>
-  </si>
-  <si>
-    <t>VIPNET d.o.o.</t>
-  </si>
-  <si>
-    <t>81793146560</t>
-  </si>
-  <si>
-    <t>Hrvatski Telekom d.d</t>
-  </si>
-  <si>
     <t>placeni_iznos_racuna</t>
+  </si>
+  <si>
+    <t>datum_od</t>
+  </si>
+  <si>
+    <t>datum_do</t>
+  </si>
+  <si>
+    <t>naziv</t>
+  </si>
+  <si>
+    <t>oib</t>
+  </si>
+  <si>
+    <t>mjesto</t>
+  </si>
+  <si>
+    <t>ulica</t>
+  </si>
+  <si>
+    <t>broj</t>
+  </si>
+  <si>
+    <t>oznaka_poreznog_broja</t>
+  </si>
+  <si>
+    <t>porezni_broj</t>
+  </si>
+  <si>
+    <t>naziv_kupca</t>
+  </si>
+  <si>
+    <t>broj_izdanog_racuna</t>
+  </si>
+  <si>
+    <t>opz_ukupan_iznos_racuna_s_pdv</t>
+  </si>
+  <si>
+    <t>opz_ukupan_iznos_pdv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ _H_R_K"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -189,14 +148,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -477,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,6 +449,8 @@
     <col min="6" max="6" width="9.5" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
@@ -495,153 +458,81 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>42651</v>
-      </c>
-      <c r="B2" s="2">
-        <v>42653</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2">
-        <v>94398799148</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2">
-        <v>47</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="2">
-        <v>42653</v>
-      </c>
-      <c r="O2" s="2">
-        <v>42653</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="H2" s="6"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>29524210204</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -651,111 +542,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="A2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>42439</v>
-      </c>
-      <c r="C2" s="2">
-        <v>42439</v>
-      </c>
-      <c r="D2">
-        <v>10000</v>
-      </c>
-      <c r="E2">
-        <v>500</v>
-      </c>
-      <c r="F2">
-        <v>1500</v>
-      </c>
-      <c r="G2" s="4">
-        <v>29524210204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>42470</v>
-      </c>
-      <c r="C3" s="2">
-        <v>42470</v>
-      </c>
-      <c r="D3">
-        <v>20000</v>
-      </c>
-      <c r="E3">
-        <v>200</v>
-      </c>
-      <c r="F3">
-        <v>2000</v>
-      </c>
-      <c r="G3" s="4">
-        <v>29524210204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>42014</v>
-      </c>
-      <c r="C4" s="2">
-        <v>42379</v>
-      </c>
-      <c r="D4">
-        <v>50000</v>
-      </c>
-      <c r="E4">
-        <v>1500</v>
-      </c>
-      <c r="F4">
-        <v>3200</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>33</v>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Izradeno dodavanje kupaca preko excel tablice (poseban view, posebne funkcije, odvojeno od opz-stat-1), izradene funkcije unutar controller-a za dodavanje kupaca preko excel tablice, izradene funkcije unutar model-a kupac, izradena forma koja se prikazuje sve kupce koji imaju konflit u nazivu (isti oib, pdv identifikacijski broj ili ostali brojevi, a razlicit naziv), izmijenjene sablone excel tablica
</commit_message>
<xml_diff>
--- a/app/assets/Sablona_za_nenaplacena_potrazivanja.xlsx
+++ b/app/assets/Sablona_za_nenaplacena_potrazivanja.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="3760" yWindow="460" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Zaglavlje" sheetId="1" r:id="rId1"/>
-    <sheet name="Kupci" sheetId="2" r:id="rId2"/>
-    <sheet name="Racuni" sheetId="3" r:id="rId3"/>
+    <sheet name="Racuni" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>email</t>
   </si>
@@ -34,9 +33,6 @@
     <t>na_dan</t>
   </si>
   <si>
-    <t>nisu_naplaceni_do</t>
-  </si>
-  <si>
     <t>datum_izdanog_racuna</t>
   </si>
   <si>
@@ -55,12 +51,6 @@
     <t>placeni_iznos_racuna</t>
   </si>
   <si>
-    <t>datum_od</t>
-  </si>
-  <si>
-    <t>datum_do</t>
-  </si>
-  <si>
     <t>naziv</t>
   </si>
   <si>
@@ -74,15 +64,6 @@
   </si>
   <si>
     <t>broj</t>
-  </si>
-  <si>
-    <t>oznaka_poreznog_broja</t>
-  </si>
-  <si>
-    <t>porezni_broj</t>
-  </si>
-  <si>
-    <t>naziv_kupca</t>
   </si>
   <si>
     <t>broj_izdanog_racuna</t>
@@ -148,7 +129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -158,6 +139,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -436,73 +418,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="H2" s="6"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F2" s="6"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -511,44 +483,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A2:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="A2:G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -558,28 +499,334 @@
     <col min="7" max="7" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>7</v>
-      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F60" s="9"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F67" s="9"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F73"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F74"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F75"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F76" s="9"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F77"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F78"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F79"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F80"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F81"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F82"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F83"/>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F88"/>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F89"/>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F90"/>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F91"/>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F92"/>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F93"/>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F95"/>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F96"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F97"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F98"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F99"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F100"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F101"/>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F102"/>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F103"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>